<commit_message>
Add Bay of Funday catch
</commit_message>
<xml_diff>
--- a/data/Table_4_Bradford_2016.xlsx
+++ b/data/Table_4_Bradford_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJR_sturgeon\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\~\SJR_sturgeon\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,18 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Catch</t>
+    <t>NB_Fundy</t>
+  </si>
+  <si>
+    <t>NS_Fundy</t>
+  </si>
+  <si>
+    <t>SJR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,1035 +353,1803 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B128"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1880</v>
       </c>
       <c r="B2">
         <v>273.29000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1881</v>
       </c>
       <c r="B3">
         <v>205.68</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1882</v>
       </c>
       <c r="B4">
         <v>128.97999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1883</v>
       </c>
       <c r="B5">
         <v>56.83</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1884</v>
       </c>
       <c r="B6">
         <v>29.11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1885</v>
       </c>
       <c r="B7">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1886</v>
       </c>
       <c r="B8">
         <v>7.38</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1887</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1888</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1889</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1890</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1891</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1892</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1893</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1894</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1895</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1896</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1897</v>
       </c>
       <c r="B19">
         <v>11.34</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1898</v>
       </c>
       <c r="B20">
         <v>9.07</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1899</v>
       </c>
       <c r="B21">
         <v>5.44</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1900</v>
       </c>
       <c r="B22">
         <v>4.54</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1901</v>
       </c>
       <c r="B23">
         <v>0.91</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1902</v>
       </c>
       <c r="B24">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1903</v>
       </c>
       <c r="B25">
         <v>2.72</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1904</v>
       </c>
       <c r="B26">
         <v>2.72</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1905</v>
       </c>
       <c r="B27">
         <v>4.38</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1906</v>
       </c>
       <c r="B28">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1907</v>
       </c>
       <c r="B29">
         <v>4.3099999999999996</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1908</v>
       </c>
       <c r="B30">
         <v>2.2269999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1909</v>
       </c>
       <c r="B31">
         <v>5.58</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1910</v>
       </c>
       <c r="B32">
         <v>7.48</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>1.81</v>
+      </c>
+      <c r="D32">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1911</v>
       </c>
       <c r="B33">
         <v>2.1800000000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>0.91</v>
+      </c>
+      <c r="D33">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1912</v>
       </c>
       <c r="B34">
         <v>4.17</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>2.63</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1913</v>
       </c>
       <c r="B35">
         <v>3.18</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>4.76</v>
+      </c>
+      <c r="D35">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1914</v>
       </c>
       <c r="B36">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>2.72</v>
+      </c>
+      <c r="D36">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1915</v>
       </c>
       <c r="B37">
         <v>3.95</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1916</v>
       </c>
       <c r="B38">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>0.91</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1917</v>
       </c>
       <c r="B39">
         <v>1.41</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>0.68</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1918</v>
       </c>
       <c r="B40">
         <v>2.09</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>0.91</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1919</v>
       </c>
       <c r="B41">
         <v>3.18</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>0.91</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1920</v>
       </c>
       <c r="B42">
         <v>3.63</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1921</v>
       </c>
       <c r="B43">
         <v>4.49</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1922</v>
       </c>
       <c r="B44">
         <v>5.03</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1923</v>
       </c>
       <c r="B45">
         <v>4.54</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1924</v>
       </c>
       <c r="B46">
         <v>2.99</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1925</v>
       </c>
       <c r="B47">
         <v>1.91</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1926</v>
       </c>
       <c r="B48">
         <v>2.59</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1927</v>
       </c>
       <c r="B49">
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1928</v>
       </c>
       <c r="B50">
         <v>3.04</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1929</v>
       </c>
       <c r="B51">
         <v>1.32</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1930</v>
       </c>
       <c r="B52">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>10.210000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1931</v>
       </c>
       <c r="B53">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>0.95</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1932</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1933</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1934</v>
       </c>
       <c r="B56">
         <v>2.72</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1935</v>
       </c>
       <c r="B57">
         <v>3.63</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1936</v>
       </c>
       <c r="B58">
         <v>2.95</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1937</v>
       </c>
       <c r="B59">
         <v>2.31</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1938</v>
       </c>
       <c r="B60">
         <v>1.63</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1939</v>
       </c>
       <c r="B61">
         <v>1.22</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1940</v>
       </c>
       <c r="B62">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1941</v>
       </c>
       <c r="B63">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1942</v>
       </c>
       <c r="B64">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>0.59</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1943</v>
       </c>
       <c r="B65">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1944</v>
       </c>
       <c r="B66">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>1.36</v>
+      </c>
+      <c r="D66">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1945</v>
       </c>
       <c r="B67">
         <v>1.59</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>0.77</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1946</v>
       </c>
       <c r="B68">
         <v>2.81</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>1.36</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1947</v>
       </c>
       <c r="B69">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>0.45</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1948</v>
       </c>
       <c r="B70">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>1.36</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1949</v>
       </c>
       <c r="B71">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>0.91</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1950</v>
       </c>
       <c r="B72">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1951</v>
       </c>
       <c r="B73">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>0.45</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1952</v>
       </c>
       <c r="B74">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1953</v>
       </c>
       <c r="B75">
         <v>3.18</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>0.45</v>
+      </c>
+      <c r="D75">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1954</v>
       </c>
       <c r="B76">
         <v>3.63</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>1.81</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1955</v>
       </c>
       <c r="B77">
         <v>4.08</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>0.45</v>
+      </c>
+      <c r="D77">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1956</v>
       </c>
       <c r="B78">
         <v>2.27</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1957</v>
       </c>
       <c r="B79">
         <v>2.72</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>3.18</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1958</v>
       </c>
       <c r="B80">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>3.18</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1959</v>
       </c>
       <c r="B81">
         <v>3.63</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>1.81</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1960</v>
       </c>
       <c r="B82">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>2.27</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1961</v>
       </c>
       <c r="B83">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>3.18</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1962</v>
       </c>
       <c r="B84">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>0.91</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1963</v>
       </c>
       <c r="B85">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>0.45</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1964</v>
       </c>
       <c r="B86">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>0.91</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1965</v>
       </c>
       <c r="B87">
         <v>2.27</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>2.27</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1966</v>
       </c>
       <c r="B88">
         <v>2.72</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1967</v>
       </c>
       <c r="B89">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1968</v>
       </c>
       <c r="B90">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>4.08</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1969</v>
       </c>
       <c r="B91">
         <v>8.16</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1970</v>
       </c>
       <c r="B92">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>0.91</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1971</v>
       </c>
       <c r="B93">
         <v>3.63</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1972</v>
       </c>
       <c r="B94">
         <v>7.26</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>0.45</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1973</v>
       </c>
       <c r="B95">
         <v>4.08</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>0.91</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1974</v>
       </c>
       <c r="B96">
         <v>2.72</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <v>1.81</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1975</v>
       </c>
       <c r="B97">
         <v>3.18</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <v>1.36</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1976</v>
       </c>
       <c r="B98">
         <v>8.98</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>1.34</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1977</v>
       </c>
       <c r="B99">
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <v>0.11</v>
+      </c>
+      <c r="D99">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1978</v>
       </c>
       <c r="B100">
         <v>7.19</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>0.05</v>
+      </c>
+      <c r="D100">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1979</v>
       </c>
       <c r="B101">
         <v>14.57</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1980</v>
       </c>
       <c r="B102">
         <v>23.06</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1981</v>
       </c>
       <c r="B103">
         <v>11.19</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <v>1.57</v>
+      </c>
+      <c r="D103">
+        <v>7.02</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1982</v>
       </c>
       <c r="B104">
         <v>11.16</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <v>0.03</v>
+      </c>
+      <c r="D104">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1983</v>
       </c>
       <c r="B105">
         <v>13.88</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <v>0.32</v>
+      </c>
+      <c r="D105">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1984</v>
       </c>
       <c r="B106">
         <v>16.96</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <v>0.21</v>
+      </c>
+      <c r="D106">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1985</v>
       </c>
       <c r="B107">
         <v>16.02</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <v>14.03</v>
+      </c>
+      <c r="D107">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1986</v>
       </c>
       <c r="B108">
         <v>14.09</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108">
+        <v>3.45</v>
+      </c>
+      <c r="D108">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1987</v>
       </c>
       <c r="B109">
         <v>7.08</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109">
+        <v>3.07</v>
+      </c>
+      <c r="D109">
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1988</v>
       </c>
       <c r="B110">
         <v>40.94</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <v>3.24</v>
+      </c>
+      <c r="D110">
+        <v>9.2899999999999991</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1989</v>
       </c>
       <c r="B111">
         <v>40.46</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C111">
+        <v>0.11</v>
+      </c>
+      <c r="D111">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1990</v>
       </c>
       <c r="B112">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C112">
+        <v>0.92</v>
+      </c>
+      <c r="D112">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1991</v>
       </c>
       <c r="B113">
         <v>9.4600000000000009</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C113">
+        <v>0.08</v>
+      </c>
+      <c r="D113">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1992</v>
       </c>
       <c r="B114">
         <v>9.6199999999999992</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C114">
+        <v>0.3</v>
+      </c>
+      <c r="D114">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1993</v>
       </c>
       <c r="B115">
         <v>4.93</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C115">
+        <v>0.09</v>
+      </c>
+      <c r="D115">
+        <v>8.86</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1994</v>
       </c>
       <c r="B116">
         <v>10.210000000000001</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <v>0.06</v>
+      </c>
+      <c r="D116">
+        <v>6.04</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1995</v>
       </c>
       <c r="B117">
         <v>10.57</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <v>0.19</v>
+      </c>
+      <c r="D117">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1996</v>
       </c>
       <c r="B118">
         <v>13.77</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118">
+        <v>0.08</v>
+      </c>
+      <c r="D118">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1997</v>
       </c>
       <c r="B119">
         <v>11.27</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C119">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D119">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1998</v>
       </c>
       <c r="B120">
         <v>6.16</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>4.1900000000000004</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>1999</v>
       </c>
       <c r="B121">
         <v>3.23</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2000</v>
       </c>
       <c r="B122">
         <v>2.52</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2001</v>
       </c>
       <c r="B123">
         <v>10.34</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2002</v>
       </c>
       <c r="B124">
         <v>5.07</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2003</v>
       </c>
       <c r="B125">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2004</v>
       </c>
       <c r="B126">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2005</v>
       </c>
       <c r="B127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2006</v>
       </c>
       <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
         <v>0</v>
       </c>
     </row>

</xml_diff>